<commit_message>
Electron charge to mass ratio lab 2, remeasured data, still require cleaning and analyzing of the outliers. Curve fit and plots working.
</commit_message>
<xml_diff>
--- a/Electron Charge Mass/Constant_Current_data.xlsx
+++ b/Electron Charge Mass/Constant_Current_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruich\Documents\GitHub\PHY224-2025\Electron Charge Mass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDBD576-018C-491E-A897-6813DE9D8337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE046C0C-94CD-4732-B4F9-A5353158D9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9C52C153-BF04-4B84-BA27-26E2C3CE8235}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>